<commit_message>
Updated flash messages for invalid login And user not getting redirected to blank page after updating or changing location
</commit_message>
<xml_diff>
--- a/python_script/bw_billing_tracker.xlsx
+++ b/python_script/bw_billing_tracker.xlsx
@@ -468,16 +468,16 @@
         <v>Apr</v>
       </c>
       <c r="B2" t="str">
-        <v>Project</v>
+        <v>nlklkjl</v>
       </c>
       <c r="C2" t="str">
-        <v>Delta</v>
+        <v>Decommissioned</v>
       </c>
       <c r="D2" t="str">
-        <v>Live</v>
+        <v>JPDC1</v>
       </c>
       <c r="E2" t="str">
-        <v>JPDC1</v>
+        <v>B</v>
       </c>
       <c r="F2" t="str">
         <v>A</v>
@@ -488,10 +488,10 @@
       <c r="H2" t="str">
         <v>192.168.4.0/24</v>
       </c>
-      <c r="I2">
+      <c r="I2" t="str">
         <v>12</v>
       </c>
-      <c r="J2">
+      <c r="J2" t="str">
         <v>345</v>
       </c>
       <c r="K2" t="str">
@@ -500,7 +500,7 @@
       <c r="L2" t="str">
         <v>ISP4</v>
       </c>
-      <c r="M2">
+      <c r="M2" t="str">
         <v>400</v>
       </c>
       <c r="N2" t="str">
@@ -509,7 +509,7 @@
       <c r="O2" t="str">
         <v>ABC</v>
       </c>
-      <c r="P2">
+      <c r="P2" t="str">
         <v>45387</v>
       </c>
       <c r="Q2" t="str">
@@ -530,13 +530,13 @@
         <v>Project</v>
       </c>
       <c r="C3" t="str">
-        <v>Epsil</v>
+        <v>Decommissioned</v>
       </c>
       <c r="D3" t="str">
-        <v>onLive</v>
+        <v>JPDC1</v>
       </c>
       <c r="E3" t="str">
-        <v>JPDC2</v>
+        <v>B</v>
       </c>
       <c r="F3" t="str">
         <v>B</v>
@@ -547,10 +547,10 @@
       <c r="H3" t="str">
         <v>192.168.5.0/24</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="str">
         <v>345</v>
       </c>
-      <c r="J3">
+      <c r="J3" t="str">
         <v>678</v>
       </c>
       <c r="K3" t="str">
@@ -559,7 +559,7 @@
       <c r="L3" t="str">
         <v>ISP5</v>
       </c>
-      <c r="M3">
+      <c r="M3" t="str">
         <v>500</v>
       </c>
       <c r="N3" t="str">
@@ -568,7 +568,7 @@
       <c r="O3" t="str">
         <v>XYZ</v>
       </c>
-      <c r="P3">
+      <c r="P3" t="str">
         <v>45430</v>
       </c>
       <c r="Q3" t="str">

</xml_diff>

<commit_message>
Color coding is added
</commit_message>
<xml_diff>
--- a/python_script/bw_billing_tracker.xlsx
+++ b/python_script/bw_billing_tracker.xlsx
@@ -530,7 +530,7 @@
         <v>Project</v>
       </c>
       <c r="C3" t="str">
-        <v>Decommissioned</v>
+        <v>Live</v>
       </c>
       <c r="D3" t="str">
         <v>JPDC1</v>
@@ -578,7 +578,7 @@
         <v>No</v>
       </c>
       <c r="S3" t="str">
-        <v>Quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea</v>
+        <v>downgrade</v>
       </c>
     </row>
     <row r="4">
@@ -696,7 +696,7 @@
         <v>No</v>
       </c>
       <c r="S5" t="str">
-        <v>Alpha Test Adding</v>
+        <v>upgrade</v>
       </c>
     </row>
   </sheetData>

</xml_diff>